<commit_message>
log4j codes are added
</commit_message>
<xml_diff>
--- a/src/test/java/DataFromExcel/TestData.xlsx
+++ b/src/test/java/DataFromExcel/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10609"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ddroy\IdeaProjects\Nexxvali_QA_Codes\src\test\java\DataFromExcel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/debopriyadebroy/Documents/Developer/Nexxvali /Test_Automation_Codes/src/test/java/DataFromExcel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A9548A2-60FF-45B3-AC88-1FF5BBD6F43D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FD910DA-BB25-274F-BF43-860E41A6467E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4320" yWindow="4170" windowWidth="21630" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6020" yWindow="8400" windowWidth="21640" windowHeight="11320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -431,13 +431,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" zoomScale="259" zoomScaleNormal="259" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -445,7 +445,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -453,7 +453,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -461,7 +461,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -469,7 +469,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -477,7 +477,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -485,7 +485,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -493,7 +493,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -501,7 +501,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -509,7 +509,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -517,7 +517,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>13</v>
       </c>

</xml_diff>